<commit_message>
Added markdown list of NLP4RE tools
</commit_message>
<xml_diff>
--- a/replication/data/nlp4re-tools-data.xlsx
+++ b/replication/data/nlp4re-tools-data.xlsx
@@ -2345,8 +2345,7 @@
     <t>Extracts causes and effects from natural language requirements using a recursive neural tensor network.</t>
   </si>
   <si>
-    <t>https://github.com/
-springto/Fine-Grained-Causality-Extraction-From-NL-Requirements</t>
+    <t>https://github.com/springto/Fine-Grained-Causality-Extraction-From-NL-Requirements</t>
   </si>
   <si>
     <t>R037</t>
@@ -2373,8 +2372,7 @@
     <t>Two approaches to extract elements for constructing a domain model are proposed. (A) From a corpus of scenarios describing a specific task, typed dependencies are identified to extract domain concepts. (B) Generate domain concepts with the help of Masked Language Models, exploiting the world knowledge stored in such a model.</t>
   </si>
   <si>
-    <t>https://drive.google.com/drive/folders/
-1o7hG0N63bl5Gpuuvu5GsTFws4Hb4d4NL?usp=sharing</t>
+    <t>https://drive.google.com/drive/folders/1o7hG0N63bl5Gpuuvu5GsTFws4Hb4d4NL?usp=sharing</t>
   </si>
   <si>
     <t>Generation</t>
@@ -2828,7 +2826,7 @@
     <t>A "tool that exploits machine learning and deep learning for automatic classification of requirements from elicitation sessions and user feedback."</t>
   </si>
   <si>
-    <t xml:space="preserve">https://github.com/lmruizcar/Requirements-Collector-DL-Component and https://github.com/spanichella/Requirement-Collector-ML-Component </t>
+    <t>https://github.com/lmruizcar/Requirements-Collector-DL-Component</t>
   </si>
   <si>
     <t>R073</t>
@@ -2867,18 +2865,7 @@
     <t>Creates trace links between requirements and design models to capture design decisions.</t>
   </si>
   <si>
-    <r>
-      <rPr/>
-      <t xml:space="preserve">https://rijul5.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <color rgb="FF1155CC"/>
-        <u/>
-      </rPr>
-      <t>github.io/Domain-Modelling-Traceability/</t>
-    </r>
+    <t>https://rijul5.github.io/Domain-Modelling-Traceability/</t>
   </si>
   <si>
     <t>R076</t>
@@ -3133,7 +3120,7 @@
     <t>Takes requirements specifications as input, extracts domain relevant terms and ranks them according to their abstraction level.</t>
   </si>
   <si>
-    <t xml:space="preserve">https://ﬁgshare.com/s/9002ed3093971325a438 </t>
+    <t>https://ﬁgshare.com/s/9002ed3093971325a438</t>
   </si>
   <si>
     <t>R097</t>
@@ -3745,10 +3732,7 @@
     <t>SACMES</t>
   </si>
   <si>
-    <t xml:space="preserve"> SACMES
-learns from the natural language specifications that it processes and stores the information that
-is learnt in a conceptual model ontology and a user history knowledge database. It then uses
-the stored information to improve performance and reduce the need for human intervention</t>
+    <t>SACMES learns from the natural language specifications that it processes and stores the information that is learnt in a conceptual model ontology and a user history knowledge database. It then uses the stored information to improve performance and reduce the need for human intervention</t>
   </si>
   <si>
     <t>R147</t>
@@ -14682,7 +14666,7 @@
       <c r="P39" s="16" t="s">
         <v>773</v>
       </c>
-      <c r="Q39" s="19" t="s">
+      <c r="Q39" s="22" t="s">
         <v>774</v>
       </c>
       <c r="R39" s="16" t="b">
@@ -14812,7 +14796,7 @@
       <c r="P41" s="16" t="s">
         <v>782</v>
       </c>
-      <c r="Q41" s="19" t="s">
+      <c r="Q41" s="22" t="s">
         <v>783</v>
       </c>
       <c r="R41" s="16" t="b">
@@ -17062,7 +17046,7 @@
       <c r="P75" s="16" t="s">
         <v>930</v>
       </c>
-      <c r="Q75" s="19" t="s">
+      <c r="Q75" s="22" t="s">
         <v>931</v>
       </c>
       <c r="R75" s="16" t="b">
@@ -25492,67 +25476,70 @@
     <hyperlink r:id="rId10" ref="Q28"/>
     <hyperlink r:id="rId11" ref="Q31"/>
     <hyperlink r:id="rId12" ref="Q35"/>
-    <hyperlink r:id="rId13" ref="Q42"/>
-    <hyperlink r:id="rId14" ref="Q43"/>
-    <hyperlink r:id="rId15" ref="Q45"/>
-    <hyperlink r:id="rId16" ref="Q48"/>
-    <hyperlink r:id="rId17" ref="Q49"/>
-    <hyperlink r:id="rId18" ref="Q52"/>
-    <hyperlink r:id="rId19" ref="Q57"/>
-    <hyperlink r:id="rId20" ref="Q63"/>
-    <hyperlink r:id="rId21" ref="N68"/>
-    <hyperlink r:id="rId22" ref="Q69"/>
-    <hyperlink r:id="rId23" ref="Q78"/>
-    <hyperlink r:id="rId24" ref="Q79"/>
-    <hyperlink r:id="rId25" ref="Q82"/>
-    <hyperlink r:id="rId26" ref="Q84"/>
-    <hyperlink r:id="rId27" ref="Q88"/>
-    <hyperlink r:id="rId28" ref="Q89"/>
-    <hyperlink r:id="rId29" ref="Q96"/>
-    <hyperlink r:id="rId30" ref="Q97"/>
-    <hyperlink r:id="rId31" ref="Q98"/>
-    <hyperlink r:id="rId32" ref="Q103"/>
-    <hyperlink r:id="rId33" ref="Q105"/>
-    <hyperlink r:id="rId34" ref="Q106"/>
-    <hyperlink r:id="rId35" ref="Q110"/>
-    <hyperlink r:id="rId36" ref="Q111"/>
-    <hyperlink r:id="rId37" ref="Q115"/>
-    <hyperlink r:id="rId38" ref="Q116"/>
-    <hyperlink r:id="rId39" ref="Q119"/>
-    <hyperlink r:id="rId40" ref="Q120"/>
-    <hyperlink r:id="rId41" ref="Q121"/>
-    <hyperlink r:id="rId42" ref="Q122"/>
-    <hyperlink r:id="rId43" ref="Q125"/>
-    <hyperlink r:id="rId44" ref="Q127"/>
-    <hyperlink r:id="rId45" ref="Q128"/>
-    <hyperlink r:id="rId46" ref="Q130"/>
-    <hyperlink r:id="rId47" ref="Q132"/>
-    <hyperlink r:id="rId48" ref="Q140"/>
-    <hyperlink r:id="rId49" ref="Q142"/>
-    <hyperlink r:id="rId50" location=".X0zuUYtCRPY." ref="Q143"/>
-    <hyperlink r:id="rId51" ref="Q147"/>
-    <hyperlink r:id="rId52" ref="Q150"/>
-    <hyperlink r:id="rId53" ref="Q151"/>
-    <hyperlink r:id="rId54" ref="Q152"/>
-    <hyperlink r:id="rId55" ref="Q155"/>
-    <hyperlink r:id="rId56" ref="Q158"/>
-    <hyperlink r:id="rId57" ref="Q161"/>
-    <hyperlink r:id="rId58" ref="Q164"/>
-    <hyperlink r:id="rId59" ref="Q165"/>
-    <hyperlink r:id="rId60" ref="Q167"/>
-    <hyperlink r:id="rId61" ref="Q168"/>
-    <hyperlink r:id="rId62" ref="Q169"/>
-    <hyperlink r:id="rId63" ref="Q173"/>
-    <hyperlink r:id="rId64" ref="Q179"/>
-    <hyperlink r:id="rId65" ref="Q183"/>
-    <hyperlink r:id="rId66" ref="Q184"/>
-    <hyperlink r:id="rId67" ref="N188"/>
-    <hyperlink r:id="rId68" ref="Q188"/>
-    <hyperlink r:id="rId69" ref="Q189"/>
-    <hyperlink r:id="rId70" ref="Q201"/>
-    <hyperlink r:id="rId71" ref="Q205"/>
+    <hyperlink r:id="rId13" ref="Q39"/>
+    <hyperlink r:id="rId14" ref="Q41"/>
+    <hyperlink r:id="rId15" ref="Q42"/>
+    <hyperlink r:id="rId16" ref="Q43"/>
+    <hyperlink r:id="rId17" ref="Q45"/>
+    <hyperlink r:id="rId18" ref="Q48"/>
+    <hyperlink r:id="rId19" ref="Q49"/>
+    <hyperlink r:id="rId20" ref="Q52"/>
+    <hyperlink r:id="rId21" ref="Q57"/>
+    <hyperlink r:id="rId22" ref="Q63"/>
+    <hyperlink r:id="rId23" ref="N68"/>
+    <hyperlink r:id="rId24" ref="Q69"/>
+    <hyperlink r:id="rId25" ref="Q75"/>
+    <hyperlink r:id="rId26" ref="Q78"/>
+    <hyperlink r:id="rId27" ref="Q79"/>
+    <hyperlink r:id="rId28" ref="Q82"/>
+    <hyperlink r:id="rId29" ref="Q84"/>
+    <hyperlink r:id="rId30" ref="Q88"/>
+    <hyperlink r:id="rId31" ref="Q89"/>
+    <hyperlink r:id="rId32" ref="Q96"/>
+    <hyperlink r:id="rId33" ref="Q97"/>
+    <hyperlink r:id="rId34" ref="Q98"/>
+    <hyperlink r:id="rId35" ref="Q103"/>
+    <hyperlink r:id="rId36" ref="Q105"/>
+    <hyperlink r:id="rId37" ref="Q106"/>
+    <hyperlink r:id="rId38" ref="Q110"/>
+    <hyperlink r:id="rId39" ref="Q111"/>
+    <hyperlink r:id="rId40" ref="Q115"/>
+    <hyperlink r:id="rId41" ref="Q116"/>
+    <hyperlink r:id="rId42" ref="Q119"/>
+    <hyperlink r:id="rId43" ref="Q120"/>
+    <hyperlink r:id="rId44" ref="Q121"/>
+    <hyperlink r:id="rId45" ref="Q122"/>
+    <hyperlink r:id="rId46" ref="Q125"/>
+    <hyperlink r:id="rId47" ref="Q127"/>
+    <hyperlink r:id="rId48" ref="Q128"/>
+    <hyperlink r:id="rId49" ref="Q130"/>
+    <hyperlink r:id="rId50" ref="Q132"/>
+    <hyperlink r:id="rId51" ref="Q140"/>
+    <hyperlink r:id="rId52" ref="Q142"/>
+    <hyperlink r:id="rId53" location=".X0zuUYtCRPY." ref="Q143"/>
+    <hyperlink r:id="rId54" ref="Q147"/>
+    <hyperlink r:id="rId55" ref="Q150"/>
+    <hyperlink r:id="rId56" ref="Q151"/>
+    <hyperlink r:id="rId57" ref="Q152"/>
+    <hyperlink r:id="rId58" ref="Q155"/>
+    <hyperlink r:id="rId59" ref="Q158"/>
+    <hyperlink r:id="rId60" ref="Q161"/>
+    <hyperlink r:id="rId61" ref="Q164"/>
+    <hyperlink r:id="rId62" ref="Q165"/>
+    <hyperlink r:id="rId63" ref="Q167"/>
+    <hyperlink r:id="rId64" ref="Q168"/>
+    <hyperlink r:id="rId65" ref="Q169"/>
+    <hyperlink r:id="rId66" ref="Q173"/>
+    <hyperlink r:id="rId67" ref="Q179"/>
+    <hyperlink r:id="rId68" ref="Q183"/>
+    <hyperlink r:id="rId69" ref="Q184"/>
+    <hyperlink r:id="rId70" ref="N188"/>
+    <hyperlink r:id="rId71" ref="Q188"/>
+    <hyperlink r:id="rId72" ref="Q189"/>
+    <hyperlink r:id="rId73" ref="Q201"/>
+    <hyperlink r:id="rId74" ref="Q205"/>
   </hyperlinks>
-  <drawing r:id="rId72"/>
+  <drawing r:id="rId75"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated data sheet with additional matrix of included (not only potential) articles per venue per year
</commit_message>
<xml_diff>
--- a/replication/data/nlp4re-tools-data.xlsx
+++ b/replication/data/nlp4re-tools-data.xlsx
@@ -6,12 +6,13 @@
     <sheet state="visible" name="Articles" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Potential Articles" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="Assignments" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Venues" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Codes Release" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="Codes License" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="Codes Availability" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="Codes Activity" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="Codes Task" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="Venues (potential)" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Venues (inclusion)" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="Codes Release" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="Codes License" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="Codes Availability" sheetId="8" r:id="rId11"/>
+    <sheet state="visible" name="Codes Activity" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="Codes Task" sheetId="10" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Articles!$D$1:$D$1000</definedName>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2507" uniqueCount="1513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2534" uniqueCount="1513">
   <si>
     <t>RID</t>
   </si>
@@ -4597,7 +4598,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -4647,6 +4648,11 @@
     <font>
       <b/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -4749,7 +4755,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -4841,17 +4847,23 @@
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="6" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -4914,6 +4926,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -12171,6 +12187,163 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="13.38"/>
+    <col customWidth="1" min="2" max="2" width="50.13"/>
+    <col customWidth="1" min="3" max="3" width="5.13"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="52" t="s">
+        <v>594</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>1504</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="52" t="s">
+        <v>1455</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>1505</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="11" t="s">
+        <v>1495</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>594</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="52" t="s">
+        <v>709</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>1506</v>
+      </c>
+      <c r="C4" s="36">
+        <f>COUNTIF('Potential Articles'!W$4:W11, A4)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="52" t="s">
+        <v>580</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>1507</v>
+      </c>
+      <c r="C5" s="36">
+        <f>COUNTIF('Potential Articles'!W$4:W11, A5)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="52" t="s">
+        <v>628</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>1508</v>
+      </c>
+      <c r="C6" s="36">
+        <f>COUNTIF('Potential Articles'!W$4:W11, A6)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="52" t="s">
+        <v>869</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>1509</v>
+      </c>
+      <c r="C7" s="36">
+        <f>COUNTIF('Potential Articles'!W$4:W11, A7)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="52" t="s">
+        <v>615</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>1510</v>
+      </c>
+      <c r="C8" s="36">
+        <f>COUNTIF('Potential Articles'!W$4:W11, A8)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="52" t="s">
+        <v>823</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>1511</v>
+      </c>
+      <c r="C9" s="36">
+        <f>COUNTIF('Potential Articles'!W$4:W11, A9)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="52" t="s">
+        <v>784</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>1512</v>
+      </c>
+      <c r="C10" s="36">
+        <f>COUNTIF('Potential Articles'!W$4:W11, A10)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="11" t="s">
+        <v>1445</v>
+      </c>
+      <c r="B11" s="53"/>
+      <c r="C11" s="32">
+        <f>SUM(C4:C10)</f>
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C4:C10">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percent" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFCFE2F3"/>
+        <color rgb="FF9FC5E8"/>
+        <color rgb="FF6FA8DC"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
@@ -25441,23 +25614,23 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="M4:M205">
+      <formula1>"included,excluded,pending"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="T4:T205">
+      <formula1>'Codes License'!$A$2:$A$14</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C4:C205">
       <formula1>Assignments!$B$2:$B$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="T4:T205">
-      <formula1>'Codes License'!$A$2:$A$14</formula1>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="U4:U205">
+      <formula1>'Codes Availability'!$A$4:$A$11</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="V4:V205">
       <formula1>'Codes Activity'!$A$4:$A$10</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4:F205">
-      <formula1>Venues!$A$2:$A$13</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="M4:M205">
-      <formula1>"included,excluded,pending"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="U4:U205">
-      <formula1>'Codes Availability'!$A$4:$A$11</formula1>
+      <formula1>'Venues (potential)'!$A$2:$A$13</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="W4:W205">
       <formula1>'Codes Task'!$A$4:$A$10</formula1>
@@ -26136,12 +26309,481 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="1" max="1" width="9.13"/>
+    <col customWidth="1" min="2" max="2" width="46.0"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="34"/>
+      <c r="B1" s="9" t="s">
+        <v>584</v>
+      </c>
+      <c r="C1" s="9">
+        <v>2019.0</v>
+      </c>
+      <c r="D1" s="9">
+        <v>2020.0</v>
+      </c>
+      <c r="E1" s="9">
+        <v>2021.0</v>
+      </c>
+      <c r="F1" s="9">
+        <v>2022.0</v>
+      </c>
+      <c r="G1" s="9">
+        <v>2023.0</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>1445</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="35" t="s">
+        <v>792</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>1446</v>
+      </c>
+      <c r="C2" s="37">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A2)*('Potential Articles'!$E:$E=C$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>13</v>
+      </c>
+      <c r="D2" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A2)*('Potential Articles'!$E:$E=D$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>12</v>
+      </c>
+      <c r="E2" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A2)*('Potential Articles'!$E:$E=E$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>13</v>
+      </c>
+      <c r="F2" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A2)*('Potential Articles'!$E:$E=F$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>7</v>
+      </c>
+      <c r="G2" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A2)*('Potential Articles'!$E:$E=G$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="27">
+        <f t="shared" ref="H2:H13" si="1">SUM(C2:G2)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="35" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>1447</v>
+      </c>
+      <c r="C3" s="37">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A3)*('Potential Articles'!$E:$E=C$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>2</v>
+      </c>
+      <c r="D3" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A3)*('Potential Articles'!$E:$E=D$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A3)*('Potential Articles'!$E:$E=E$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A3)*('Potential Articles'!$E:$E=F$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>3</v>
+      </c>
+      <c r="G3" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A3)*('Potential Articles'!$E:$E=G$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>2</v>
+      </c>
+      <c r="H3" s="27">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="35" t="s">
+        <v>1346</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>1448</v>
+      </c>
+      <c r="C4" s="37">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A4)*('Potential Articles'!$E:$E=C$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>1</v>
+      </c>
+      <c r="D4" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A4)*('Potential Articles'!$E:$E=D$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>1</v>
+      </c>
+      <c r="E4" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A4)*('Potential Articles'!$E:$E=E$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>2</v>
+      </c>
+      <c r="F4" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A4)*('Potential Articles'!$E:$E=F$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>2</v>
+      </c>
+      <c r="G4" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A4)*('Potential Articles'!$E:$E=G$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="27">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="35" t="s">
+        <v>697</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>1449</v>
+      </c>
+      <c r="C5" s="37">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A5)*('Potential Articles'!$E:$E=C$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>3</v>
+      </c>
+      <c r="D5" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A5)*('Potential Articles'!$E:$E=D$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>6</v>
+      </c>
+      <c r="E5" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A5)*('Potential Articles'!$E:$E=E$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>6</v>
+      </c>
+      <c r="F5" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A5)*('Potential Articles'!$E:$E=F$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>2</v>
+      </c>
+      <c r="G5" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A5)*('Potential Articles'!$E:$E=G$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="27">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="35" t="s">
+        <v>1408</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="37">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A6)*('Potential Articles'!$E:$E=C$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A6)*('Potential Articles'!$E:$E=D$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>2</v>
+      </c>
+      <c r="E6" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A6)*('Potential Articles'!$E:$E=E$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A6)*('Potential Articles'!$E:$E=F$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>1</v>
+      </c>
+      <c r="G6" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A6)*('Potential Articles'!$E:$E=G$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>1</v>
+      </c>
+      <c r="H6" s="27">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="35" t="s">
+        <v>1192</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="C7" s="37">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A7)*('Potential Articles'!$E:$E=C$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A7)*('Potential Articles'!$E:$E=D$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>3</v>
+      </c>
+      <c r="E7" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A7)*('Potential Articles'!$E:$E=E$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A7)*('Potential Articles'!$E:$E=F$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>2</v>
+      </c>
+      <c r="G7" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A7)*('Potential Articles'!$E:$E=G$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="27">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="35" t="s">
+        <v>1220</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>1450</v>
+      </c>
+      <c r="C8" s="37">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A8)*('Potential Articles'!$E:$E=C$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A8)*('Potential Articles'!$E:$E=D$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>2</v>
+      </c>
+      <c r="E8" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A8)*('Potential Articles'!$E:$E=E$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A8)*('Potential Articles'!$E:$E=F$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A8)*('Potential Articles'!$E:$E=G$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="27">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="35" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>494</v>
+      </c>
+      <c r="C9" s="37">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A9)*('Potential Articles'!$E:$E=C$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A9)*('Potential Articles'!$E:$E=D$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A9)*('Potential Articles'!$E:$E=E$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>1</v>
+      </c>
+      <c r="F9" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A9)*('Potential Articles'!$E:$E=F$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>4</v>
+      </c>
+      <c r="G9" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A9)*('Potential Articles'!$E:$E=G$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>5</v>
+      </c>
+      <c r="H9" s="27">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="35" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>558</v>
+      </c>
+      <c r="C10" s="37">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A10)*('Potential Articles'!$E:$E=C$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>3</v>
+      </c>
+      <c r="D10" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A10)*('Potential Articles'!$E:$E=D$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>1</v>
+      </c>
+      <c r="E10" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A10)*('Potential Articles'!$E:$E=E$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>3</v>
+      </c>
+      <c r="F10" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A10)*('Potential Articles'!$E:$E=F$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>2</v>
+      </c>
+      <c r="G10" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A10)*('Potential Articles'!$E:$E=G$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>2</v>
+      </c>
+      <c r="H10" s="27">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="35" t="s">
+        <v>605</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>1451</v>
+      </c>
+      <c r="C11" s="37">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A11)*('Potential Articles'!$E:$E=C$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>1</v>
+      </c>
+      <c r="D11" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A11)*('Potential Articles'!$E:$E=D$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>1</v>
+      </c>
+      <c r="E11" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A11)*('Potential Articles'!$E:$E=E$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>5</v>
+      </c>
+      <c r="F11" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A11)*('Potential Articles'!$E:$E=F$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>2</v>
+      </c>
+      <c r="G11" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A11)*('Potential Articles'!$E:$E=G$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>1</v>
+      </c>
+      <c r="H11" s="27">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="35" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>1452</v>
+      </c>
+      <c r="C12" s="37">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A12)*('Potential Articles'!$E:$E=C$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A12)*('Potential Articles'!$E:$E=D$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>1</v>
+      </c>
+      <c r="E12" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A12)*('Potential Articles'!$E:$E=E$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A12)*('Potential Articles'!$E:$E=F$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>1</v>
+      </c>
+      <c r="G12" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A12)*('Potential Articles'!$E:$E=G$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>2</v>
+      </c>
+      <c r="H12" s="27">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="35" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>1453</v>
+      </c>
+      <c r="C13" s="37">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A13)*('Potential Articles'!$E:$E=C$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A13)*('Potential Articles'!$E:$E=D$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>1</v>
+      </c>
+      <c r="E13" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A13)*('Potential Articles'!$E:$E=E$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>3</v>
+      </c>
+      <c r="F13" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A13)*('Potential Articles'!$E:$E=F$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="38">
+        <f>SUMPRODUCT(('Potential Articles'!$F:$F=$A13)*('Potential Articles'!$E:$E=G$1)*('Potential Articles'!$M:$M="included"))</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="27">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" ht="15.0" customHeight="1">
+      <c r="A14" s="34"/>
+      <c r="B14" s="9" t="s">
+        <v>1445</v>
+      </c>
+      <c r="C14" s="32">
+        <f t="shared" ref="C14:H14" si="2">SUM(C2:C13)</f>
+        <v>23</v>
+      </c>
+      <c r="D14" s="32">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="E14" s="32">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="F14" s="32">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="G14" s="32">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="H14" s="32">
+        <f t="shared" si="2"/>
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C2:G13">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percent" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFCFE2F3"/>
+        <color rgb="FF9FC5E8"/>
+        <color rgb="FF6FA8DC"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
     <col customWidth="1" min="2" max="2" width="37.63"/>
     <col customWidth="1" min="3" max="3" width="5.13"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="39" t="s">
         <v>594</v>
       </c>
       <c r="B1" s="16" t="s">
@@ -26149,7 +26791,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="39" t="s">
         <v>1455</v>
       </c>
       <c r="B2" s="16" t="s">
@@ -26168,7 +26810,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="39" t="s">
         <v>596</v>
       </c>
       <c r="B4" s="14" t="s">
@@ -26180,7 +26822,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="39" t="s">
         <v>597</v>
       </c>
       <c r="B5" s="14" t="s">
@@ -26192,7 +26834,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="39" t="s">
         <v>1462</v>
       </c>
       <c r="B6" s="14" t="s">
@@ -26204,7 +26846,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="39" t="s">
         <v>658</v>
       </c>
       <c r="B7" s="14" t="s">
@@ -26219,7 +26861,7 @@
       <c r="A8" s="9" t="s">
         <v>1445</v>
       </c>
-      <c r="B8" s="38"/>
+      <c r="B8" s="40"/>
       <c r="C8" s="32">
         <f>SUM(C4:C7)</f>
         <v>202</v>
@@ -26234,7 +26876,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -26261,10 +26903,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="39" t="s">
         <v>644</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="41" t="s">
         <v>1466</v>
       </c>
       <c r="C2" s="36">
@@ -26273,10 +26915,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="39" t="s">
         <v>1467</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="42" t="s">
         <v>1468</v>
       </c>
       <c r="C3" s="36">
@@ -26285,7 +26927,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="39" t="s">
         <v>658</v>
       </c>
       <c r="B4" s="14" t="s">
@@ -26297,10 +26939,10 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="39" t="s">
         <v>725</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="42" t="s">
         <v>1470</v>
       </c>
       <c r="C5" s="36">
@@ -26309,7 +26951,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="39" t="s">
         <v>625</v>
       </c>
       <c r="B6" s="14" t="s">
@@ -26321,10 +26963,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="39" t="s">
         <v>692</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="41" t="s">
         <v>1472</v>
       </c>
       <c r="C7" s="36">
@@ -26333,10 +26975,10 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="39" t="s">
         <v>796</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="42" t="s">
         <v>1473</v>
       </c>
       <c r="C8" s="36">
@@ -26345,10 +26987,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="39" t="s">
         <v>612</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="42" t="s">
         <v>1474</v>
       </c>
       <c r="C9" s="36">
@@ -26357,10 +26999,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="39" t="s">
         <v>686</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="42" t="s">
         <v>1475</v>
       </c>
       <c r="C10" s="36">
@@ -26369,10 +27011,10 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="39" t="s">
         <v>1273</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="42" t="s">
         <v>1476</v>
       </c>
       <c r="C11" s="36">
@@ -26381,10 +27023,10 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="39" t="s">
         <v>1369</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="41" t="s">
         <v>1477</v>
       </c>
       <c r="C12" s="36">
@@ -26393,10 +27035,10 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="39" t="s">
         <v>1478</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="41" t="s">
         <v>1479</v>
       </c>
       <c r="C13" s="36">
@@ -26431,7 +27073,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -26446,7 +27088,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="39" t="s">
         <v>594</v>
       </c>
       <c r="B1" s="16" t="s">
@@ -26454,7 +27096,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="39" t="s">
         <v>1455</v>
       </c>
       <c r="B2" s="16" t="s">
@@ -26473,7 +27115,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="43" t="s">
         <v>693</v>
       </c>
       <c r="B4" s="16" t="s">
@@ -26485,7 +27127,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="44" t="s">
         <v>613</v>
       </c>
       <c r="B5" s="16" t="s">
@@ -26497,7 +27139,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="45" t="s">
         <v>659</v>
       </c>
       <c r="B6" s="16" t="s">
@@ -26509,7 +27151,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="46" t="s">
         <v>714</v>
       </c>
       <c r="B7" s="16" t="s">
@@ -26521,7 +27163,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="47" t="s">
         <v>838</v>
       </c>
       <c r="B8" s="16" t="s">
@@ -26533,7 +27175,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="48" t="s">
         <v>626</v>
       </c>
       <c r="B9" s="16" t="s">
@@ -26545,7 +27187,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="49" t="s">
         <v>1489</v>
       </c>
       <c r="B10" s="16" t="s">
@@ -26557,7 +27199,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="50" t="s">
         <v>1491</v>
       </c>
       <c r="B11" s="16" t="s">
@@ -26572,7 +27214,7 @@
       <c r="A12" s="9" t="s">
         <v>1445</v>
       </c>
-      <c r="B12" s="49"/>
+      <c r="B12" s="51"/>
       <c r="C12" s="32">
         <f>SUM(C4:C11)</f>
         <v>126</v>
@@ -26584,162 +27226,6 @@
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:C11">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percent" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFCFE2F3"/>
-        <color rgb="FF9FC5E8"/>
-        <color rgb="FF6FA8DC"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="2" max="2" width="68.88"/>
-    <col customWidth="1" min="3" max="3" width="5.13"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="50" t="s">
-        <v>594</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>1493</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="50" t="s">
-        <v>1455</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>1494</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="11" t="s">
-        <v>1495</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>594</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>1459</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="50" t="s">
-        <v>627</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>1496</v>
-      </c>
-      <c r="C4" s="36">
-        <f>COUNTIF('Potential Articles'!V$4:V11, A4)</f>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="50" t="s">
-        <v>660</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>1497</v>
-      </c>
-      <c r="C5" s="36">
-        <f>COUNTIF('Potential Articles'!V$4:V11, A5)</f>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="50" t="s">
-        <v>694</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>1498</v>
-      </c>
-      <c r="C6" s="36">
-        <f>COUNTIF('Potential Articles'!V$4:V11, A6)</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="50" t="s">
-        <v>674</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>1499</v>
-      </c>
-      <c r="C7" s="36">
-        <f>COUNTIF('Potential Articles'!V$4:V11, A7)</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="50" t="s">
-        <v>614</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>1500</v>
-      </c>
-      <c r="C8" s="36">
-        <f>COUNTIF('Potential Articles'!V$4:V11, A8)</f>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="50" t="s">
-        <v>1501</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>1502</v>
-      </c>
-      <c r="C9" s="36">
-        <f>COUNTIF('Potential Articles'!V$4:V11, A9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="50" t="s">
-        <v>715</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>1503</v>
-      </c>
-      <c r="C10" s="36">
-        <f>COUNTIF('Potential Articles'!V$4:V11, A10)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="11" t="s">
-        <v>1445</v>
-      </c>
-      <c r="B11" s="51"/>
-      <c r="C11" s="32">
-        <f>SUM(C4:C10)</f>
-        <v>127</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-  </mergeCells>
-  <conditionalFormatting sqref="C4:C10">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -26765,25 +27251,24 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="13.38"/>
-    <col customWidth="1" min="2" max="2" width="50.13"/>
+    <col customWidth="1" min="2" max="2" width="68.88"/>
     <col customWidth="1" min="3" max="3" width="5.13"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="52" t="s">
         <v>594</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>1504</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="52" t="s">
         <v>1455</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>1505</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="3">
@@ -26798,94 +27283,94 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="50" t="s">
-        <v>709</v>
+      <c r="A4" s="52" t="s">
+        <v>627</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>1506</v>
+        <v>1496</v>
       </c>
       <c r="C4" s="36">
-        <f>COUNTIF('Potential Articles'!W$4:W11, A4)</f>
-        <v>10</v>
+        <f>COUNTIF('Potential Articles'!V$4:V11, A4)</f>
+        <v>38</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="50" t="s">
-        <v>580</v>
+      <c r="A5" s="52" t="s">
+        <v>660</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>1507</v>
+        <v>1497</v>
       </c>
       <c r="C5" s="36">
-        <f>COUNTIF('Potential Articles'!W$4:W11, A5)</f>
-        <v>40</v>
+        <f>COUNTIF('Potential Articles'!V$4:V11, A5)</f>
+        <v>29</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="50" t="s">
-        <v>628</v>
+      <c r="A6" s="52" t="s">
+        <v>694</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>1508</v>
+        <v>1498</v>
       </c>
       <c r="C6" s="36">
-        <f>COUNTIF('Potential Articles'!W$4:W11, A6)</f>
-        <v>35</v>
+        <f>COUNTIF('Potential Articles'!V$4:V11, A6)</f>
+        <v>18</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="50" t="s">
-        <v>869</v>
+      <c r="A7" s="52" t="s">
+        <v>674</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>1509</v>
+        <v>1499</v>
       </c>
       <c r="C7" s="36">
-        <f>COUNTIF('Potential Articles'!W$4:W11, A7)</f>
-        <v>11</v>
+        <f>COUNTIF('Potential Articles'!V$4:V11, A7)</f>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="50" t="s">
-        <v>615</v>
+      <c r="A8" s="52" t="s">
+        <v>614</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>1510</v>
+        <v>1500</v>
       </c>
       <c r="C8" s="36">
-        <f>COUNTIF('Potential Articles'!W$4:W11, A8)</f>
-        <v>19</v>
+        <f>COUNTIF('Potential Articles'!V$4:V11, A8)</f>
+        <v>26</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="50" t="s">
-        <v>823</v>
+      <c r="A9" s="52" t="s">
+        <v>1501</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>1511</v>
+        <v>1502</v>
       </c>
       <c r="C9" s="36">
-        <f>COUNTIF('Potential Articles'!W$4:W11, A9)</f>
-        <v>4</v>
+        <f>COUNTIF('Potential Articles'!V$4:V11, A9)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="50" t="s">
-        <v>784</v>
+      <c r="A10" s="52" t="s">
+        <v>715</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>1512</v>
+        <v>1503</v>
       </c>
       <c r="C10" s="36">
-        <f>COUNTIF('Potential Articles'!W$4:W11, A10)</f>
-        <v>8</v>
+        <f>COUNTIF('Potential Articles'!V$4:V11, A10)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="11" t="s">
         <v>1445</v>
       </c>
-      <c r="B11" s="51"/>
+      <c r="B11" s="53"/>
       <c r="C11" s="32">
         <f>SUM(C4:C10)</f>
         <v>127</v>

</xml_diff>

<commit_message>
Corrected minor data point issue
</commit_message>
<xml_diff>
--- a/replication/data/nlp4re-tools-data.xlsx
+++ b/replication/data/nlp4re-tools-data.xlsx
@@ -16,6 +16,7 @@
   </sheets>
   <definedNames>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Articles!$D$1:$D$1000</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'Potential Articles'!$V$3:$W$205</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
@@ -21733,7 +21734,7 @@
         <v>0</v>
       </c>
       <c r="T144" s="16" t="s">
-        <v>658</v>
+        <v>625</v>
       </c>
       <c r="U144" s="16" t="s">
         <v>626</v>
@@ -25596,6 +25597,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="$V$3:$W$205"/>
   <mergeCells count="5">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:F1"/>
@@ -26910,7 +26912,7 @@
         <v>1466</v>
       </c>
       <c r="C2" s="36">
-        <f>IF(NOT(ISBLANK(A2)), COUNTIF('Potential Articles'!T:T, A2), "")</f>
+        <f>IF(NOT(ISBLANK(A2)), COUNTIF('Potential Articles'!T$4:T14, A2), "")</f>
         <v>11</v>
       </c>
     </row>
@@ -26922,7 +26924,7 @@
         <v>1468</v>
       </c>
       <c r="C3" s="36">
-        <f>IF(NOT(ISBLANK(A3)), COUNTIF('Potential Articles'!T:T, A3), "")</f>
+        <f>IF(NOT(ISBLANK(A3)), COUNTIF('Potential Articles'!T$4:T14, A3), "")</f>
         <v>0</v>
       </c>
     </row>
@@ -26934,8 +26936,8 @@
         <v>1469</v>
       </c>
       <c r="C4" s="36">
-        <f>IF(NOT(ISBLANK(A4)), COUNTIF('Potential Articles'!T:T, A4), "")</f>
-        <v>29</v>
+        <f>IF(NOT(ISBLANK(A4)), COUNTIF('Potential Articles'!T$4:T14, A4), "")</f>
+        <v>28</v>
       </c>
     </row>
     <row r="5">
@@ -26946,7 +26948,7 @@
         <v>1470</v>
       </c>
       <c r="C5" s="36">
-        <f>IF(NOT(ISBLANK(A5)), COUNTIF('Potential Articles'!T:T, A5), "")</f>
+        <f>IF(NOT(ISBLANK(A5)), COUNTIF('Potential Articles'!T$4:T14, A5), "")</f>
         <v>6</v>
       </c>
     </row>
@@ -26958,8 +26960,8 @@
         <v>1471</v>
       </c>
       <c r="C6" s="36">
-        <f>IF(NOT(ISBLANK(A6)), COUNTIF('Potential Articles'!T:T, A6), "")</f>
-        <v>60</v>
+        <f>IF(NOT(ISBLANK(A6)), COUNTIF('Potential Articles'!T$4:T14, A6), "")</f>
+        <v>61</v>
       </c>
     </row>
     <row r="7">
@@ -26970,7 +26972,7 @@
         <v>1472</v>
       </c>
       <c r="C7" s="36">
-        <f>IF(NOT(ISBLANK(A7)), COUNTIF('Potential Articles'!T:T, A7), "")</f>
+        <f>IF(NOT(ISBLANK(A7)), COUNTIF('Potential Articles'!T$4:T14, A7), "")</f>
         <v>7</v>
       </c>
     </row>
@@ -26982,7 +26984,7 @@
         <v>1473</v>
       </c>
       <c r="C8" s="36">
-        <f>IF(NOT(ISBLANK(A8)), COUNTIF('Potential Articles'!T:T, A8), "")</f>
+        <f>IF(NOT(ISBLANK(A8)), COUNTIF('Potential Articles'!T$4:T14, A8), "")</f>
         <v>6</v>
       </c>
     </row>
@@ -26994,7 +26996,7 @@
         <v>1474</v>
       </c>
       <c r="C9" s="36">
-        <f>IF(NOT(ISBLANK(A9)), COUNTIF('Potential Articles'!T:T, A9), "")</f>
+        <f>IF(NOT(ISBLANK(A9)), COUNTIF('Potential Articles'!T$4:T14, A9), "")</f>
         <v>4</v>
       </c>
     </row>
@@ -27006,7 +27008,7 @@
         <v>1475</v>
       </c>
       <c r="C10" s="36">
-        <f>IF(NOT(ISBLANK(A10)), COUNTIF('Potential Articles'!T:T, A10), "")</f>
+        <f>IF(NOT(ISBLANK(A10)), COUNTIF('Potential Articles'!T$4:T14, A10), "")</f>
         <v>1</v>
       </c>
     </row>
@@ -27018,7 +27020,7 @@
         <v>1476</v>
       </c>
       <c r="C11" s="36">
-        <f>IF(NOT(ISBLANK(A11)), COUNTIF('Potential Articles'!T:T, A11), "")</f>
+        <f>IF(NOT(ISBLANK(A11)), COUNTIF('Potential Articles'!T$4:T14, A11), "")</f>
         <v>1</v>
       </c>
     </row>
@@ -27030,7 +27032,7 @@
         <v>1477</v>
       </c>
       <c r="C12" s="36">
-        <f>IF(NOT(ISBLANK(A12)), COUNTIF('Potential Articles'!T:T, A12), "")</f>
+        <f>IF(NOT(ISBLANK(A12)), COUNTIF('Potential Articles'!T$4:T14, A12), "")</f>
         <v>1</v>
       </c>
     </row>
@@ -27042,7 +27044,7 @@
         <v>1479</v>
       </c>
       <c r="C13" s="36">
-        <f>IF(NOT(ISBLANK(A13)), COUNTIF('Potential Articles'!T:T, A13), "")</f>
+        <f>IF(NOT(ISBLANK(A13)), COUNTIF('Potential Articles'!T$4:T14, A13), "")</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>